<commit_message>
Inicializar_SCTimer no genera picos en 0% pero no funciona con la otra salida. SCTimer_Init basado en 2 Outs independientes. Agrega MdE y capturas de picos
</commit_message>
<xml_diff>
--- a/Senoidal.xlsx
+++ b/Senoidal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t xml:space="preserve">1 Intervalo pi/10</t>
   </si>
@@ -108,6 +108,9 @@
     <t xml:space="preserve">R C real</t>
   </si>
   <si>
+    <t xml:space="preserve">10000</t>
+  </si>
+  <si>
     <t xml:space="preserve">[us]</t>
   </si>
   <si>
@@ -131,7 +134,7 @@
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -161,6 +164,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF2E3436"/>
+      <name val="Cantarell"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="14"/>
@@ -274,7 +283,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,6 +297,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,13 +382,13 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF2E3436"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -412,8 +425,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.351073535673013"/>
-          <c:y val="0.0206017891027379"/>
+          <c:x val="0.351076773330089"/>
+          <c:y val="0.0206036508223387"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -562,11 +575,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="28311976"/>
-        <c:axId val="56324854"/>
+        <c:axId val="76877978"/>
+        <c:axId val="13850664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28311976"/>
+        <c:axId val="76877978"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,13 +622,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56324854"/>
+        <c:crossAx val="13850664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56324854"/>
+        <c:axId val="13850664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +671,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28311976"/>
+        <c:crossAx val="76877978"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -686,7 +699,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -724,8 +737,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.351083149565443"/>
-          <c:y val="0.0206933619994625"/>
+          <c:x val="0.351041058571707"/>
+          <c:y val="0.020695215911127"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -870,11 +883,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="99208307"/>
-        <c:axId val="34321990"/>
+        <c:axId val="79884733"/>
+        <c:axId val="17357111"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99208307"/>
+        <c:axId val="79884733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +930,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34321990"/>
+        <c:crossAx val="17357111"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34321990"/>
+        <c:axId val="17357111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +981,568 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99208307"/>
+        <c:crossAx val="79884733"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="es-AR" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="es-AR" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:rPr>
+              <a:t>Seno</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.351076773330089"/>
+          <c:y val="0.0206036508223387"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="003e76"/>
+            </a:solidFill>
+            <a:ln cap="rnd" w="19080">
+              <a:solidFill>
+                <a:srgbClr val="003e76"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial Unicode MS"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$101:$G$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$103:$G$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.587785252292473</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.951056516295154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.951056516295154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.587785252292473</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.22464679914735E-016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="79074298"/>
+        <c:axId val="34859440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="79074298"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="bfbfbf"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="34859440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="34859440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="bfbfbf"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79074298"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="es-AR" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="es-AR" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:rPr>
+              <a:t>%Área
+</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.351041058571707"/>
+          <c:y val="0.020695215911127"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="003e76"/>
+            </a:solidFill>
+            <a:ln w="25560">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                    <a:ea typeface="Arial Unicode MS"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$107:$G$107</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$105:$G$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.303958893917744</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.795774715459477</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.983631643083466</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.795774715459477</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.303958893917744</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="0"/>
+        <c:axId val="91199567"/>
+        <c:axId val="52538085"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="91199567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="bfbfbf"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52538085"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="52538085"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="bfbfbf"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial Unicode MS"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91199567"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1007,9 +1581,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>358920</xdr:colOff>
+      <xdr:colOff>358560</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1018,7 +1592,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="257040" y="2244600"/>
-        <a:ext cx="5918400" cy="3983760"/>
+        <a:ext cx="5917320" cy="3983400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1037,9 +1611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>303120</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1047,12 +1621,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6340320" y="2225880"/>
-        <a:ext cx="5550120" cy="4018320"/>
+        <a:off x="6339600" y="2225880"/>
+        <a:ext cx="5549760" cy="4017960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>508320</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>37080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609840</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>58320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="508320" y="18081360"/>
+        <a:ext cx="5917320" cy="3983400"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238320</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>139680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>175680</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="7455600" y="18031320"/>
+        <a:ext cx="5549760" cy="4017960"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1066,10 +1700,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:GC99"/>
+  <dimension ref="A3:GC176"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A120" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J112" activeCellId="0" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1692,6 +2326,11 @@
         <v>1545.08497187474</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="str">
         <f aca="false">B8</f>
@@ -1742,7 +2381,7 @@
         <v>1000</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,48 +2424,48 @@
       <c r="M46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="4" t="n">
+      <c r="C47" s="5" t="n">
         <f aca="false">IF(D44&gt;10,100,D44)</f>
         <v>100</v>
       </c>
-      <c r="D47" s="4" t="n">
+      <c r="D47" s="5" t="n">
         <f aca="false">IF(D46&gt;10,100,IF(D46&lt;0,0,D46*10))</f>
         <v>55.791947275279</v>
       </c>
-      <c r="E47" s="4" t="n">
+      <c r="E47" s="5" t="n">
         <f aca="false">IF(E46&gt;10,100,IF(E46&lt;0,0,E46*10))</f>
         <v>0</v>
       </c>
-      <c r="F47" s="4" t="n">
+      <c r="F47" s="5" t="n">
         <f aca="false">IF(F46&gt;10,100,IF(F46&lt;0,0,F46*10))</f>
         <v>0</v>
       </c>
-      <c r="G47" s="4" t="n">
+      <c r="G47" s="5" t="n">
         <f aca="false">IF(G46&gt;10,100,IF(G46&lt;0,0,G46*10))</f>
         <v>0</v>
       </c>
-      <c r="H47" s="4" t="n">
+      <c r="H47" s="5" t="n">
         <f aca="false">IF(H46&gt;10,100,IF(H46&lt;0,0,H46*10))</f>
         <v>0</v>
       </c>
-      <c r="I47" s="4" t="n">
+      <c r="I47" s="5" t="n">
         <f aca="false">IF(I46&gt;10,100,IF(I46&lt;0,0,I46*10))</f>
         <v>0</v>
       </c>
-      <c r="J47" s="4" t="n">
+      <c r="J47" s="5" t="n">
         <f aca="false">IF(J46&gt;10,100,IF(J46&lt;0,0,J46*10))</f>
         <v>0</v>
       </c>
-      <c r="K47" s="4" t="n">
+      <c r="K47" s="5" t="n">
         <f aca="false">IF(K46&gt;10,100,IF(K46&lt;0,0,K46*10))</f>
         <v>0</v>
       </c>
-      <c r="L47" s="4" t="n">
+      <c r="L47" s="5" t="n">
         <f aca="false">IF(L46&gt;10,100,IF(L46&lt;0,0,L46*10))</f>
         <v>0</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +2517,7 @@
         <v>1000</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,48 +2559,48 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="4" t="n">
+      <c r="C52" s="5" t="n">
         <f aca="false">IF(D49&gt;10,100,D49)</f>
         <v>100</v>
       </c>
-      <c r="D52" s="4" t="n">
+      <c r="D52" s="5" t="n">
         <f aca="false">IF(D51&gt;10,100,IF(D51&lt;0,0,D51*10))</f>
         <v>100</v>
       </c>
-      <c r="E52" s="4" t="n">
+      <c r="E52" s="5" t="n">
         <f aca="false">IF(E51&gt;10,100,IF(E51&lt;0,0,E51*10))</f>
         <v>100</v>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F52" s="5" t="n">
         <f aca="false">IF(F51&gt;10,100,IF(F51&lt;0,0,F51*10))</f>
         <v>100</v>
       </c>
-      <c r="G52" s="4" t="n">
+      <c r="G52" s="5" t="n">
         <f aca="false">IF(G51&gt;10,100,IF(G51&lt;0,0,G51*10))</f>
         <v>52.125840560208</v>
       </c>
-      <c r="H52" s="4" t="n">
+      <c r="H52" s="5" t="n">
         <f aca="false">IF(H51&gt;10,100,IF(H51&lt;0,0,H51*10))</f>
         <v>0</v>
       </c>
-      <c r="I52" s="4" t="n">
+      <c r="I52" s="5" t="n">
         <f aca="false">IF(I51&gt;10,100,IF(I51&lt;0,0,I51*10))</f>
         <v>0</v>
       </c>
-      <c r="J52" s="4" t="n">
+      <c r="J52" s="5" t="n">
         <f aca="false">IF(J51&gt;10,100,IF(J51&lt;0,0,J51*10))</f>
         <v>0</v>
       </c>
-      <c r="K52" s="4" t="n">
+      <c r="K52" s="5" t="n">
         <f aca="false">IF(K51&gt;10,100,IF(K51&lt;0,0,K51*10))</f>
         <v>0</v>
       </c>
-      <c r="L52" s="4" t="n">
+      <c r="L52" s="5" t="n">
         <f aca="false">IF(L51&gt;10,100,IF(L51&lt;0,0,L51*10))</f>
         <v>0</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,7 +2652,7 @@
         <v>1000</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,48 +2695,48 @@
       <c r="M56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="4" t="n">
+      <c r="C57" s="5" t="n">
         <f aca="false">IF(D54&gt;10,100,D54)</f>
         <v>100</v>
       </c>
-      <c r="D57" s="4" t="n">
+      <c r="D57" s="5" t="n">
         <f aca="false">IF(D56&gt;10,100,IF(D56&lt;0,0,D56*10))</f>
         <v>100</v>
       </c>
-      <c r="E57" s="4" t="n">
+      <c r="E57" s="5" t="n">
         <f aca="false">IF(E56&gt;10,100,IF(E56&lt;0,0,E56*10))</f>
         <v>100</v>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F57" s="5" t="n">
         <f aca="false">IF(F56&gt;10,100,IF(F56&lt;0,0,F56*10))</f>
         <v>100</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G57" s="5" t="n">
         <f aca="false">IF(G56&gt;10,100,IF(G56&lt;0,0,G56*10))</f>
         <v>100</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="5" t="n">
         <f aca="false">IF(H56&gt;10,100,IF(H56&lt;0,0,H56*10))</f>
         <v>100</v>
       </c>
-      <c r="I57" s="4" t="n">
+      <c r="I57" s="5" t="n">
         <f aca="false">IF(I56&gt;10,100,IF(I56&lt;0,0,I56*10))</f>
         <v>100</v>
       </c>
-      <c r="J57" s="4" t="n">
+      <c r="J57" s="5" t="n">
         <f aca="false">IF(J56&gt;10,100,IF(J56&lt;0,0,J56*10))</f>
         <v>4.20250642514105</v>
       </c>
-      <c r="K57" s="4" t="n">
+      <c r="K57" s="5" t="n">
         <f aca="false">IF(K56&gt;10,100,IF(K56&lt;0,0,K56*10))</f>
         <v>0</v>
       </c>
-      <c r="L57" s="4" t="n">
+      <c r="L57" s="5" t="n">
         <f aca="false">IF(L56&gt;10,100,IF(L56&lt;0,0,L56*10))</f>
         <v>0</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,7 +2788,7 @@
         <v>1000</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,48 +2831,48 @@
       <c r="M61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="4" t="n">
+      <c r="C62" s="5" t="n">
         <f aca="false">IF(D59&gt;10,100,D59)</f>
         <v>100</v>
       </c>
-      <c r="D62" s="4" t="n">
+      <c r="D62" s="5" t="n">
         <f aca="false">IF(D61&gt;10,100,IF(D61&lt;0,0,D61*10))</f>
         <v>100</v>
       </c>
-      <c r="E62" s="4" t="n">
+      <c r="E62" s="5" t="n">
         <f aca="false">IF(E61&gt;10,100,IF(E61&lt;0,0,E61*10))</f>
         <v>100</v>
       </c>
-      <c r="F62" s="4" t="n">
+      <c r="F62" s="5" t="n">
         <f aca="false">IF(F61&gt;10,100,IF(F61&lt;0,0,F61*10))</f>
         <v>100</v>
       </c>
-      <c r="G62" s="4" t="n">
+      <c r="G62" s="5" t="n">
         <f aca="false">IF(G61&gt;10,100,IF(G61&lt;0,0,G61*10))</f>
         <v>100</v>
       </c>
-      <c r="H62" s="4" t="n">
+      <c r="H62" s="5" t="n">
         <f aca="false">IF(H61&gt;10,100,IF(H61&lt;0,0,H61*10))</f>
         <v>100</v>
       </c>
-      <c r="I62" s="4" t="n">
+      <c r="I62" s="5" t="n">
         <f aca="false">IF(I61&gt;10,100,IF(I61&lt;0,0,I61*10))</f>
         <v>100</v>
       </c>
-      <c r="J62" s="4" t="n">
+      <c r="J62" s="5" t="n">
         <f aca="false">IF(J61&gt;10,100,IF(J61&lt;0,0,J61*10))</f>
         <v>100</v>
       </c>
-      <c r="K62" s="4" t="n">
+      <c r="K62" s="5" t="n">
         <f aca="false">IF(K61&gt;10,100,IF(K61&lt;0,0,K61*10))</f>
         <v>87.346924493812</v>
       </c>
-      <c r="L62" s="4" t="n">
+      <c r="L62" s="5" t="n">
         <f aca="false">IF(L61&gt;10,100,IF(L61&lt;0,0,L61*10))</f>
         <v>0</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2924,7 @@
         <v>1000</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,48 +2967,48 @@
       <c r="M66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="4" t="n">
+      <c r="C67" s="5" t="n">
         <f aca="false">IF(D64&gt;10,100,D64)</f>
         <v>100</v>
       </c>
-      <c r="D67" s="4" t="n">
+      <c r="D67" s="5" t="n">
         <f aca="false">IF(D66&gt;10,100,IF(D66&lt;0,0,D66*10))</f>
         <v>100</v>
       </c>
-      <c r="E67" s="4" t="n">
+      <c r="E67" s="5" t="n">
         <f aca="false">IF(E66&gt;10,100,IF(E66&lt;0,0,E66*10))</f>
         <v>100</v>
       </c>
-      <c r="F67" s="4" t="n">
+      <c r="F67" s="5" t="n">
         <f aca="false">IF(F66&gt;10,100,IF(F66&lt;0,0,F66*10))</f>
         <v>100</v>
       </c>
-      <c r="G67" s="4" t="n">
+      <c r="G67" s="5" t="n">
         <f aca="false">IF(G66&gt;10,100,IF(G66&lt;0,0,G66*10))</f>
         <v>100</v>
       </c>
-      <c r="H67" s="4" t="n">
+      <c r="H67" s="5" t="n">
         <f aca="false">IF(H66&gt;10,100,IF(H66&lt;0,0,H66*10))</f>
         <v>100</v>
       </c>
-      <c r="I67" s="4" t="n">
+      <c r="I67" s="5" t="n">
         <f aca="false">IF(I66&gt;10,100,IF(I66&lt;0,0,I66*10))</f>
         <v>100</v>
       </c>
-      <c r="J67" s="4" t="n">
+      <c r="J67" s="5" t="n">
         <f aca="false">IF(J66&gt;10,100,IF(J66&lt;0,0,J66*10))</f>
         <v>100</v>
       </c>
-      <c r="K67" s="4" t="n">
+      <c r="K67" s="5" t="n">
         <f aca="false">IF(K66&gt;10,100,IF(K66&lt;0,0,K66*10))</f>
         <v>100</v>
       </c>
-      <c r="L67" s="4" t="n">
+      <c r="L67" s="5" t="n">
         <f aca="false">IF(L66&gt;10,100,IF(L66&lt;0,0,L66*10))</f>
         <v>83.631643083466</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +3060,7 @@
         <v>1000</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,48 +3103,48 @@
       <c r="M71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="4" t="n">
+      <c r="C72" s="5" t="n">
         <f aca="false">IF(D69&gt;10,100,D69)</f>
         <v>100</v>
       </c>
-      <c r="D72" s="4" t="n">
+      <c r="D72" s="5" t="n">
         <f aca="false">IF(D71&gt;10,100,IF(D71&lt;0,0,D71*10))</f>
         <v>100</v>
       </c>
-      <c r="E72" s="4" t="n">
+      <c r="E72" s="5" t="n">
         <f aca="false">IF(E71&gt;10,100,IF(E71&lt;0,0,E71*10))</f>
         <v>100</v>
       </c>
-      <c r="F72" s="4" t="n">
+      <c r="F72" s="5" t="n">
         <f aca="false">IF(F71&gt;10,100,IF(F71&lt;0,0,F71*10))</f>
         <v>100</v>
       </c>
-      <c r="G72" s="4" t="n">
+      <c r="G72" s="5" t="n">
         <f aca="false">IF(G71&gt;10,100,IF(G71&lt;0,0,G71*10))</f>
         <v>100</v>
       </c>
-      <c r="H72" s="4" t="n">
+      <c r="H72" s="5" t="n">
         <f aca="false">IF(H71&gt;10,100,IF(H71&lt;0,0,H71*10))</f>
         <v>100</v>
       </c>
-      <c r="I72" s="4" t="n">
+      <c r="I72" s="5" t="n">
         <f aca="false">IF(I71&gt;10,100,IF(I71&lt;0,0,I71*10))</f>
         <v>100</v>
       </c>
-      <c r="J72" s="4" t="n">
+      <c r="J72" s="5" t="n">
         <f aca="false">IF(J71&gt;10,100,IF(J71&lt;0,0,J71*10))</f>
         <v>100</v>
       </c>
-      <c r="K72" s="4" t="n">
+      <c r="K72" s="5" t="n">
         <f aca="false">IF(K71&gt;10,100,IF(K71&lt;0,0,K71*10))</f>
         <v>100</v>
       </c>
-      <c r="L72" s="4" t="n">
+      <c r="L72" s="5" t="n">
         <f aca="false">IF(L71&gt;10,100,IF(L71&lt;0,0,L71*10))</f>
         <v>83.631643083466</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,7 +3196,7 @@
         <v>1000</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2600,48 +3239,48 @@
       <c r="M76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="4" t="n">
+      <c r="C77" s="5" t="n">
         <f aca="false">IF(D74&gt;10,100,D74)</f>
         <v>100</v>
       </c>
-      <c r="D77" s="4" t="n">
+      <c r="D77" s="5" t="n">
         <f aca="false">IF(D76&gt;10,100,IF(D76&lt;0,0,D76*10))</f>
         <v>100</v>
       </c>
-      <c r="E77" s="4" t="n">
+      <c r="E77" s="5" t="n">
         <f aca="false">IF(E76&gt;10,100,IF(E76&lt;0,0,E76*10))</f>
         <v>100</v>
       </c>
-      <c r="F77" s="4" t="n">
+      <c r="F77" s="5" t="n">
         <f aca="false">IF(F76&gt;10,100,IF(F76&lt;0,0,F76*10))</f>
         <v>100</v>
       </c>
-      <c r="G77" s="4" t="n">
+      <c r="G77" s="5" t="n">
         <f aca="false">IF(G76&gt;10,100,IF(G76&lt;0,0,G76*10))</f>
         <v>100</v>
       </c>
-      <c r="H77" s="4" t="n">
+      <c r="H77" s="5" t="n">
         <f aca="false">IF(H76&gt;10,100,IF(H76&lt;0,0,H76*10))</f>
         <v>100</v>
       </c>
-      <c r="I77" s="4" t="n">
+      <c r="I77" s="5" t="n">
         <f aca="false">IF(I76&gt;10,100,IF(I76&lt;0,0,I76*10))</f>
         <v>100</v>
       </c>
-      <c r="J77" s="4" t="n">
+      <c r="J77" s="5" t="n">
         <f aca="false">IF(J76&gt;10,100,IF(J76&lt;0,0,J76*10))</f>
         <v>100</v>
       </c>
-      <c r="K77" s="4" t="n">
+      <c r="K77" s="5" t="n">
         <f aca="false">IF(K76&gt;10,100,IF(K76&lt;0,0,K76*10))</f>
         <v>87.346924493812</v>
       </c>
-      <c r="L77" s="4" t="n">
+      <c r="L77" s="5" t="n">
         <f aca="false">IF(L76&gt;10,100,IF(L76&lt;0,0,L76*10))</f>
         <v>0</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2693,7 +3332,7 @@
         <v>1000</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,48 +3375,48 @@
       <c r="M81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="4" t="n">
+      <c r="C82" s="5" t="n">
         <f aca="false">IF(D79&gt;10,100,D79)</f>
         <v>100</v>
       </c>
-      <c r="D82" s="4" t="n">
+      <c r="D82" s="5" t="n">
         <f aca="false">IF(D81&gt;10,100,IF(D81&lt;0,0,D81*10))</f>
         <v>100</v>
       </c>
-      <c r="E82" s="4" t="n">
+      <c r="E82" s="5" t="n">
         <f aca="false">IF(E81&gt;10,100,IF(E81&lt;0,0,E81*10))</f>
         <v>100</v>
       </c>
-      <c r="F82" s="4" t="n">
+      <c r="F82" s="5" t="n">
         <f aca="false">IF(F81&gt;10,100,IF(F81&lt;0,0,F81*10))</f>
         <v>100</v>
       </c>
-      <c r="G82" s="4" t="n">
+      <c r="G82" s="5" t="n">
         <f aca="false">IF(G81&gt;10,100,IF(G81&lt;0,0,G81*10))</f>
         <v>100</v>
       </c>
-      <c r="H82" s="4" t="n">
+      <c r="H82" s="5" t="n">
         <f aca="false">IF(H81&gt;10,100,IF(H81&lt;0,0,H81*10))</f>
         <v>100</v>
       </c>
-      <c r="I82" s="4" t="n">
+      <c r="I82" s="5" t="n">
         <f aca="false">IF(I81&gt;10,100,IF(I81&lt;0,0,I81*10))</f>
         <v>100</v>
       </c>
-      <c r="J82" s="4" t="n">
+      <c r="J82" s="5" t="n">
         <f aca="false">IF(J81&gt;10,100,IF(J81&lt;0,0,J81*10))</f>
         <v>4.20250642514105</v>
       </c>
-      <c r="K82" s="4" t="n">
+      <c r="K82" s="5" t="n">
         <f aca="false">IF(K81&gt;10,100,IF(K81&lt;0,0,K81*10))</f>
         <v>0</v>
       </c>
-      <c r="L82" s="4" t="n">
+      <c r="L82" s="5" t="n">
         <f aca="false">IF(L81&gt;10,100,IF(L81&lt;0,0,L81*10))</f>
         <v>0</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,7 +3468,7 @@
         <v>1000</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2872,48 +3511,48 @@
       <c r="M86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="4" t="n">
+      <c r="C87" s="5" t="n">
         <f aca="false">IF(D84&gt;10,100,D84)</f>
         <v>100</v>
       </c>
-      <c r="D87" s="4" t="n">
+      <c r="D87" s="5" t="n">
         <f aca="false">IF(D86&gt;10,100,IF(D86&lt;0,0,D86*10))</f>
         <v>100</v>
       </c>
-      <c r="E87" s="4" t="n">
+      <c r="E87" s="5" t="n">
         <f aca="false">IF(E86&gt;10,100,IF(E86&lt;0,0,E86*10))</f>
         <v>100</v>
       </c>
-      <c r="F87" s="4" t="n">
+      <c r="F87" s="5" t="n">
         <f aca="false">IF(F86&gt;10,100,IF(F86&lt;0,0,F86*10))</f>
         <v>100</v>
       </c>
-      <c r="G87" s="4" t="n">
+      <c r="G87" s="5" t="n">
         <f aca="false">IF(G86&gt;10,100,IF(G86&lt;0,0,G86*10))</f>
         <v>52.125840560209</v>
       </c>
-      <c r="H87" s="4" t="n">
+      <c r="H87" s="5" t="n">
         <f aca="false">IF(H86&gt;10,100,IF(H86&lt;0,0,H86*10))</f>
         <v>0</v>
       </c>
-      <c r="I87" s="4" t="n">
+      <c r="I87" s="5" t="n">
         <f aca="false">IF(I86&gt;10,100,IF(I86&lt;0,0,I86*10))</f>
         <v>0</v>
       </c>
-      <c r="J87" s="4" t="n">
+      <c r="J87" s="5" t="n">
         <f aca="false">IF(J86&gt;10,100,IF(J86&lt;0,0,J86*10))</f>
         <v>0</v>
       </c>
-      <c r="K87" s="4" t="n">
+      <c r="K87" s="5" t="n">
         <f aca="false">IF(K86&gt;10,100,IF(K86&lt;0,0,K86*10))</f>
         <v>0</v>
       </c>
-      <c r="L87" s="4" t="n">
+      <c r="L87" s="5" t="n">
         <f aca="false">IF(L86&gt;10,100,IF(L86&lt;0,0,L86*10))</f>
         <v>0</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +3604,7 @@
         <v>1000</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,53 +3647,53 @@
       <c r="M91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="4" t="n">
+      <c r="C92" s="5" t="n">
         <f aca="false">IF(D89&gt;10,100,D89)</f>
         <v>100</v>
       </c>
-      <c r="D92" s="4" t="n">
+      <c r="D92" s="5" t="n">
         <f aca="false">IF(D91&gt;10,100,IF(D91&lt;0,0,D91*10))</f>
         <v>55.791947275279</v>
       </c>
-      <c r="E92" s="4" t="n">
+      <c r="E92" s="5" t="n">
         <f aca="false">IF(E91&gt;10,100,IF(E91&lt;0,0,E91*10))</f>
         <v>0</v>
       </c>
-      <c r="F92" s="4" t="n">
+      <c r="F92" s="5" t="n">
         <f aca="false">IF(F91&gt;10,100,IF(F91&lt;0,0,F91*10))</f>
         <v>0</v>
       </c>
-      <c r="G92" s="4" t="n">
+      <c r="G92" s="5" t="n">
         <f aca="false">IF(G91&gt;10,100,IF(G91&lt;0,0,G91*10))</f>
         <v>0</v>
       </c>
-      <c r="H92" s="4" t="n">
+      <c r="H92" s="5" t="n">
         <f aca="false">IF(H91&gt;10,100,IF(H91&lt;0,0,H91*10))</f>
         <v>0</v>
       </c>
-      <c r="I92" s="4" t="n">
+      <c r="I92" s="5" t="n">
         <f aca="false">IF(I91&gt;10,100,IF(I91&lt;0,0,I91*10))</f>
         <v>0</v>
       </c>
-      <c r="J92" s="4" t="n">
+      <c r="J92" s="5" t="n">
         <f aca="false">IF(J91&gt;10,100,IF(J91&lt;0,0,J91*10))</f>
         <v>0</v>
       </c>
-      <c r="K92" s="4" t="n">
+      <c r="K92" s="5" t="n">
         <f aca="false">IF(K91&gt;10,100,IF(K91&lt;0,0,K91*10))</f>
         <v>0</v>
       </c>
-      <c r="L92" s="4" t="n">
+      <c r="L92" s="5" t="n">
         <f aca="false">IF(L91&gt;10,100,IF(L91&lt;0,0,L91*10))</f>
         <v>0</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C96" s="3" t="n">
         <f aca="false">C47</f>
@@ -3459,556 +4098,1560 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C97" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C97" s="6" t="n">
         <f aca="false">C96</f>
         <v>100</v>
       </c>
-      <c r="D97" s="5" t="n">
+      <c r="D97" s="6" t="n">
         <f aca="false">D96</f>
         <v>55.791947275279</v>
       </c>
-      <c r="E97" s="5" t="n">
+      <c r="E97" s="6" t="n">
         <f aca="false">E96</f>
         <v>0</v>
       </c>
-      <c r="F97" s="5" t="n">
+      <c r="F97" s="6" t="n">
         <f aca="false">F96</f>
         <v>0</v>
       </c>
-      <c r="G97" s="5" t="n">
+      <c r="G97" s="6" t="n">
         <f aca="false">G96</f>
         <v>0</v>
       </c>
-      <c r="H97" s="5" t="n">
+      <c r="H97" s="6" t="n">
         <f aca="false">H96</f>
         <v>0</v>
       </c>
-      <c r="I97" s="5" t="n">
+      <c r="I97" s="6" t="n">
         <f aca="false">I96</f>
         <v>0</v>
       </c>
-      <c r="J97" s="5" t="n">
+      <c r="J97" s="6" t="n">
         <f aca="false">J96</f>
         <v>0</v>
       </c>
-      <c r="K97" s="5" t="n">
+      <c r="K97" s="6" t="n">
         <f aca="false">K96</f>
         <v>0</v>
       </c>
-      <c r="L97" s="5" t="n">
+      <c r="L97" s="6" t="n">
         <f aca="false">L96</f>
         <v>0</v>
       </c>
-      <c r="M97" s="5" t="n">
+      <c r="M97" s="6" t="n">
         <f aca="false">M96</f>
         <v>100</v>
       </c>
-      <c r="N97" s="5" t="n">
+      <c r="N97" s="6" t="n">
         <f aca="false">N96</f>
         <v>100</v>
       </c>
-      <c r="O97" s="5" t="n">
+      <c r="O97" s="6" t="n">
         <f aca="false">O96</f>
         <v>100</v>
       </c>
-      <c r="P97" s="5" t="n">
+      <c r="P97" s="6" t="n">
         <f aca="false">P96</f>
         <v>100</v>
       </c>
-      <c r="Q97" s="5" t="n">
+      <c r="Q97" s="6" t="n">
         <f aca="false">Q96</f>
         <v>52.125840560208</v>
       </c>
-      <c r="R97" s="5" t="n">
+      <c r="R97" s="6" t="n">
         <f aca="false">R96</f>
         <v>0</v>
       </c>
-      <c r="S97" s="5" t="n">
+      <c r="S97" s="6" t="n">
         <f aca="false">S96</f>
         <v>0</v>
       </c>
-      <c r="T97" s="5" t="n">
+      <c r="T97" s="6" t="n">
         <f aca="false">T96</f>
         <v>0</v>
       </c>
-      <c r="U97" s="5" t="n">
+      <c r="U97" s="6" t="n">
         <f aca="false">U96</f>
         <v>0</v>
       </c>
-      <c r="V97" s="5" t="n">
+      <c r="V97" s="6" t="n">
         <f aca="false">V96</f>
         <v>0</v>
       </c>
-      <c r="W97" s="5" t="n">
+      <c r="W97" s="6" t="n">
         <f aca="false">W96</f>
         <v>100</v>
       </c>
-      <c r="X97" s="5" t="n">
+      <c r="X97" s="6" t="n">
         <f aca="false">X96</f>
         <v>100</v>
       </c>
-      <c r="Y97" s="5" t="n">
+      <c r="Y97" s="6" t="n">
         <f aca="false">Y96</f>
         <v>100</v>
       </c>
-      <c r="Z97" s="5" t="n">
+      <c r="Z97" s="6" t="n">
         <f aca="false">Z96</f>
         <v>100</v>
       </c>
-      <c r="AA97" s="5" t="n">
+      <c r="AA97" s="6" t="n">
         <f aca="false">AA96</f>
         <v>100</v>
       </c>
-      <c r="AB97" s="5" t="n">
+      <c r="AB97" s="6" t="n">
         <f aca="false">AB96</f>
         <v>100</v>
       </c>
-      <c r="AC97" s="5" t="n">
+      <c r="AC97" s="6" t="n">
         <f aca="false">AC96</f>
         <v>100</v>
       </c>
-      <c r="AD97" s="5" t="n">
+      <c r="AD97" s="6" t="n">
         <f aca="false">AD96</f>
         <v>4.20250642514105</v>
       </c>
-      <c r="AE97" s="5" t="n">
+      <c r="AE97" s="6" t="n">
         <f aca="false">AE96</f>
         <v>0</v>
       </c>
-      <c r="AF97" s="5" t="n">
+      <c r="AF97" s="6" t="n">
         <f aca="false">AF96</f>
         <v>0</v>
       </c>
-      <c r="AG97" s="5" t="n">
+      <c r="AG97" s="6" t="n">
         <f aca="false">AG96</f>
         <v>100</v>
       </c>
-      <c r="AH97" s="5" t="n">
+      <c r="AH97" s="6" t="n">
         <f aca="false">AH96</f>
         <v>100</v>
       </c>
-      <c r="AI97" s="5" t="n">
+      <c r="AI97" s="6" t="n">
         <f aca="false">AI96</f>
         <v>100</v>
       </c>
-      <c r="AJ97" s="5" t="n">
+      <c r="AJ97" s="6" t="n">
         <f aca="false">AJ96</f>
         <v>100</v>
       </c>
-      <c r="AK97" s="5" t="n">
+      <c r="AK97" s="6" t="n">
         <f aca="false">AK96</f>
         <v>100</v>
       </c>
-      <c r="AL97" s="5" t="n">
+      <c r="AL97" s="6" t="n">
         <f aca="false">AL96</f>
         <v>100</v>
       </c>
-      <c r="AM97" s="5" t="n">
+      <c r="AM97" s="6" t="n">
         <f aca="false">AM96</f>
         <v>100</v>
       </c>
-      <c r="AN97" s="5" t="n">
+      <c r="AN97" s="6" t="n">
         <f aca="false">AN96</f>
         <v>100</v>
       </c>
-      <c r="AO97" s="5" t="n">
+      <c r="AO97" s="6" t="n">
         <f aca="false">AO96</f>
         <v>87.346924493812</v>
       </c>
-      <c r="AP97" s="5" t="n">
+      <c r="AP97" s="6" t="n">
         <f aca="false">AP96</f>
         <v>0</v>
       </c>
-      <c r="AQ97" s="5" t="n">
+      <c r="AQ97" s="6" t="n">
         <f aca="false">AQ96</f>
         <v>100</v>
       </c>
-      <c r="AR97" s="5" t="n">
+      <c r="AR97" s="6" t="n">
         <f aca="false">AR96</f>
         <v>100</v>
       </c>
-      <c r="AS97" s="5" t="n">
+      <c r="AS97" s="6" t="n">
         <f aca="false">AS96</f>
         <v>100</v>
       </c>
-      <c r="AT97" s="5" t="n">
+      <c r="AT97" s="6" t="n">
         <f aca="false">AT96</f>
         <v>100</v>
       </c>
-      <c r="AU97" s="5" t="n">
+      <c r="AU97" s="6" t="n">
         <f aca="false">AU96</f>
         <v>100</v>
       </c>
-      <c r="AV97" s="5" t="n">
+      <c r="AV97" s="6" t="n">
         <f aca="false">AV96</f>
         <v>100</v>
       </c>
-      <c r="AW97" s="5" t="n">
+      <c r="AW97" s="6" t="n">
         <f aca="false">AW96</f>
         <v>100</v>
       </c>
-      <c r="AX97" s="5" t="n">
+      <c r="AX97" s="6" t="n">
         <f aca="false">AX96</f>
         <v>100</v>
       </c>
-      <c r="AY97" s="5" t="n">
+      <c r="AY97" s="6" t="n">
         <f aca="false">AY96</f>
         <v>100</v>
       </c>
-      <c r="AZ97" s="5" t="n">
+      <c r="AZ97" s="6" t="n">
         <f aca="false">AZ96</f>
         <v>83.631643083466</v>
       </c>
-      <c r="BA97" s="5" t="n">
+      <c r="BA97" s="6" t="n">
         <f aca="false">BA96</f>
         <v>100</v>
       </c>
-      <c r="BB97" s="5" t="n">
+      <c r="BB97" s="6" t="n">
         <f aca="false">BB96</f>
         <v>100</v>
       </c>
-      <c r="BC97" s="5" t="n">
+      <c r="BC97" s="6" t="n">
         <f aca="false">BC96</f>
         <v>100</v>
       </c>
-      <c r="BD97" s="5" t="n">
+      <c r="BD97" s="6" t="n">
         <f aca="false">BD96</f>
         <v>100</v>
       </c>
-      <c r="BE97" s="5" t="n">
+      <c r="BE97" s="6" t="n">
         <f aca="false">BE96</f>
         <v>100</v>
       </c>
-      <c r="BF97" s="5" t="n">
+      <c r="BF97" s="6" t="n">
         <f aca="false">BF96</f>
         <v>100</v>
       </c>
-      <c r="BG97" s="5" t="n">
+      <c r="BG97" s="6" t="n">
         <f aca="false">BG96</f>
         <v>100</v>
       </c>
-      <c r="BH97" s="5" t="n">
+      <c r="BH97" s="6" t="n">
         <f aca="false">BH96</f>
         <v>100</v>
       </c>
-      <c r="BI97" s="5" t="n">
+      <c r="BI97" s="6" t="n">
         <f aca="false">BI96</f>
         <v>100</v>
       </c>
-      <c r="BJ97" s="5" t="n">
+      <c r="BJ97" s="6" t="n">
         <f aca="false">BJ96</f>
         <v>83.631643083466</v>
       </c>
-      <c r="BK97" s="5" t="n">
+      <c r="BK97" s="6" t="n">
         <f aca="false">BK96</f>
         <v>100</v>
       </c>
-      <c r="BL97" s="5" t="n">
+      <c r="BL97" s="6" t="n">
         <f aca="false">BL96</f>
         <v>100</v>
       </c>
-      <c r="BM97" s="5" t="n">
+      <c r="BM97" s="6" t="n">
         <f aca="false">BM96</f>
         <v>100</v>
       </c>
-      <c r="BN97" s="5" t="n">
+      <c r="BN97" s="6" t="n">
         <f aca="false">BN96</f>
         <v>100</v>
       </c>
-      <c r="BO97" s="5" t="n">
+      <c r="BO97" s="6" t="n">
         <f aca="false">BO96</f>
         <v>100</v>
       </c>
-      <c r="BP97" s="5" t="n">
+      <c r="BP97" s="6" t="n">
         <f aca="false">BP96</f>
         <v>100</v>
       </c>
-      <c r="BQ97" s="5" t="n">
+      <c r="BQ97" s="6" t="n">
         <f aca="false">BQ96</f>
         <v>100</v>
       </c>
-      <c r="BR97" s="5" t="n">
+      <c r="BR97" s="6" t="n">
         <f aca="false">BR96</f>
         <v>100</v>
       </c>
-      <c r="BS97" s="5" t="n">
+      <c r="BS97" s="6" t="n">
         <f aca="false">BS96</f>
         <v>87.346924493812</v>
       </c>
-      <c r="BT97" s="5" t="n">
+      <c r="BT97" s="6" t="n">
         <f aca="false">BT96</f>
         <v>0</v>
       </c>
-      <c r="BU97" s="5" t="n">
+      <c r="BU97" s="6" t="n">
         <f aca="false">BU96</f>
         <v>100</v>
       </c>
-      <c r="BV97" s="5" t="n">
+      <c r="BV97" s="6" t="n">
         <f aca="false">BV96</f>
         <v>100</v>
       </c>
-      <c r="BW97" s="5" t="n">
+      <c r="BW97" s="6" t="n">
         <f aca="false">BW96</f>
         <v>100</v>
       </c>
-      <c r="BX97" s="5" t="n">
+      <c r="BX97" s="6" t="n">
         <f aca="false">BX96</f>
         <v>100</v>
       </c>
-      <c r="BY97" s="5" t="n">
+      <c r="BY97" s="6" t="n">
         <f aca="false">BY96</f>
         <v>100</v>
       </c>
-      <c r="BZ97" s="5" t="n">
+      <c r="BZ97" s="6" t="n">
         <f aca="false">BZ96</f>
         <v>100</v>
       </c>
-      <c r="CA97" s="5" t="n">
+      <c r="CA97" s="6" t="n">
         <f aca="false">CA96</f>
         <v>100</v>
       </c>
-      <c r="CB97" s="5" t="n">
+      <c r="CB97" s="6" t="n">
         <f aca="false">CB96</f>
         <v>4.20250642514105</v>
       </c>
-      <c r="CC97" s="5" t="n">
+      <c r="CC97" s="6" t="n">
         <f aca="false">CC96</f>
         <v>0</v>
       </c>
-      <c r="CD97" s="5" t="n">
+      <c r="CD97" s="6" t="n">
         <f aca="false">CD96</f>
         <v>0</v>
       </c>
-      <c r="CE97" s="5" t="n">
+      <c r="CE97" s="6" t="n">
         <f aca="false">CE96</f>
         <v>100</v>
       </c>
-      <c r="CF97" s="5" t="n">
+      <c r="CF97" s="6" t="n">
         <f aca="false">CF96</f>
         <v>100</v>
       </c>
-      <c r="CG97" s="5" t="n">
+      <c r="CG97" s="6" t="n">
         <f aca="false">CG96</f>
         <v>100</v>
       </c>
-      <c r="CH97" s="5" t="n">
+      <c r="CH97" s="6" t="n">
         <f aca="false">CH96</f>
         <v>100</v>
       </c>
-      <c r="CI97" s="5" t="n">
+      <c r="CI97" s="6" t="n">
         <f aca="false">CI96</f>
         <v>52.125840560209</v>
       </c>
-      <c r="CJ97" s="5" t="n">
+      <c r="CJ97" s="6" t="n">
         <f aca="false">CJ96</f>
         <v>0</v>
       </c>
-      <c r="CK97" s="5" t="n">
+      <c r="CK97" s="6" t="n">
         <f aca="false">CK96</f>
         <v>0</v>
       </c>
-      <c r="CL97" s="5" t="n">
+      <c r="CL97" s="6" t="n">
         <f aca="false">CL96</f>
         <v>0</v>
       </c>
-      <c r="CM97" s="5" t="n">
+      <c r="CM97" s="6" t="n">
         <f aca="false">CM96</f>
         <v>0</v>
       </c>
-      <c r="CN97" s="5" t="n">
+      <c r="CN97" s="6" t="n">
         <f aca="false">CN96</f>
         <v>0</v>
       </c>
-      <c r="CO97" s="5" t="n">
+      <c r="CO97" s="6" t="n">
         <f aca="false">CO96</f>
         <v>100</v>
       </c>
-      <c r="CP97" s="5" t="n">
+      <c r="CP97" s="6" t="n">
         <f aca="false">CP96</f>
         <v>55.791947275279</v>
       </c>
-      <c r="CQ97" s="5" t="n">
+      <c r="CQ97" s="6" t="n">
         <f aca="false">CQ96</f>
         <v>0</v>
       </c>
-      <c r="CR97" s="5" t="n">
+      <c r="CR97" s="6" t="n">
         <f aca="false">CR96</f>
         <v>0</v>
       </c>
-      <c r="CS97" s="5" t="n">
+      <c r="CS97" s="6" t="n">
         <f aca="false">CS96</f>
         <v>0</v>
       </c>
-      <c r="CT97" s="5" t="n">
+      <c r="CT97" s="6" t="n">
         <f aca="false">CT96</f>
         <v>0</v>
       </c>
-      <c r="CU97" s="5" t="n">
+      <c r="CU97" s="6" t="n">
         <f aca="false">CU96</f>
         <v>0</v>
       </c>
-      <c r="CV97" s="5" t="n">
+      <c r="CV97" s="6" t="n">
         <f aca="false">CV96</f>
         <v>0</v>
       </c>
-      <c r="CW97" s="5" t="n">
+      <c r="CW97" s="6" t="n">
         <f aca="false">CW96</f>
         <v>0</v>
       </c>
-      <c r="CX97" s="5" t="n">
+      <c r="CX97" s="6" t="n">
         <f aca="false">CX96</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="J98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="O98" s="5"/>
+      <c r="C98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="O98" s="6"/>
       <c r="P98" s="1"/>
-      <c r="Q98" s="5"/>
-      <c r="R98" s="5"/>
-      <c r="T98" s="5"/>
-      <c r="V98" s="5"/>
-      <c r="W98" s="5"/>
-      <c r="Y98" s="5"/>
-      <c r="AA98" s="5"/>
-      <c r="AB98" s="5"/>
-      <c r="AD98" s="5"/>
-      <c r="AF98" s="5"/>
-      <c r="AG98" s="5"/>
-      <c r="AI98" s="5"/>
-      <c r="AK98" s="5"/>
-      <c r="AL98" s="5"/>
-      <c r="AN98" s="5"/>
-      <c r="AP98" s="5"/>
-      <c r="AQ98" s="5"/>
-      <c r="AS98" s="5"/>
-      <c r="AU98" s="5"/>
-      <c r="AV98" s="5"/>
-      <c r="AX98" s="5"/>
-      <c r="AZ98" s="5"/>
-      <c r="BA98" s="5"/>
-      <c r="BC98" s="5"/>
-      <c r="BE98" s="5"/>
-      <c r="BF98" s="5"/>
-      <c r="BH98" s="5"/>
-      <c r="BJ98" s="5"/>
-      <c r="BK98" s="5"/>
-      <c r="BM98" s="5"/>
-      <c r="BO98" s="5"/>
-      <c r="BP98" s="5"/>
-      <c r="BR98" s="5"/>
-      <c r="BT98" s="5"/>
-      <c r="BU98" s="5"/>
-      <c r="BW98" s="5"/>
-      <c r="BY98" s="5"/>
-      <c r="BZ98" s="5"/>
-      <c r="CB98" s="5"/>
-      <c r="CD98" s="5"/>
-      <c r="CE98" s="5"/>
-      <c r="CG98" s="5"/>
-      <c r="CI98" s="5"/>
-      <c r="CJ98" s="5"/>
-      <c r="CL98" s="5"/>
-      <c r="CN98" s="5"/>
-      <c r="CO98" s="5"/>
-      <c r="CQ98" s="5"/>
-      <c r="CS98" s="5"/>
-      <c r="CT98" s="5"/>
-      <c r="CV98" s="5"/>
-      <c r="CX98" s="5"/>
-      <c r="CY98" s="5"/>
+      <c r="Q98" s="6"/>
+      <c r="R98" s="6"/>
+      <c r="T98" s="6"/>
+      <c r="V98" s="6"/>
+      <c r="W98" s="6"/>
+      <c r="Y98" s="6"/>
+      <c r="AA98" s="6"/>
+      <c r="AB98" s="6"/>
+      <c r="AD98" s="6"/>
+      <c r="AF98" s="6"/>
+      <c r="AG98" s="6"/>
+      <c r="AI98" s="6"/>
+      <c r="AK98" s="6"/>
+      <c r="AL98" s="6"/>
+      <c r="AN98" s="6"/>
+      <c r="AP98" s="6"/>
+      <c r="AQ98" s="6"/>
+      <c r="AS98" s="6"/>
+      <c r="AU98" s="6"/>
+      <c r="AV98" s="6"/>
+      <c r="AX98" s="6"/>
+      <c r="AZ98" s="6"/>
+      <c r="BA98" s="6"/>
+      <c r="BC98" s="6"/>
+      <c r="BE98" s="6"/>
+      <c r="BF98" s="6"/>
+      <c r="BH98" s="6"/>
+      <c r="BJ98" s="6"/>
+      <c r="BK98" s="6"/>
+      <c r="BM98" s="6"/>
+      <c r="BO98" s="6"/>
+      <c r="BP98" s="6"/>
+      <c r="BR98" s="6"/>
+      <c r="BT98" s="6"/>
+      <c r="BU98" s="6"/>
+      <c r="BW98" s="6"/>
+      <c r="BY98" s="6"/>
+      <c r="BZ98" s="6"/>
+      <c r="CB98" s="6"/>
+      <c r="CD98" s="6"/>
+      <c r="CE98" s="6"/>
+      <c r="CG98" s="6"/>
+      <c r="CI98" s="6"/>
+      <c r="CJ98" s="6"/>
+      <c r="CL98" s="6"/>
+      <c r="CN98" s="6"/>
+      <c r="CO98" s="6"/>
+      <c r="CQ98" s="6"/>
+      <c r="CS98" s="6"/>
+      <c r="CT98" s="6"/>
+      <c r="CV98" s="6"/>
+      <c r="CX98" s="6"/>
+      <c r="CY98" s="6"/>
       <c r="CZ98" s="1"/>
-      <c r="DA98" s="5"/>
+      <c r="DA98" s="6"/>
       <c r="DB98" s="1"/>
-      <c r="DC98" s="5"/>
-      <c r="DD98" s="5"/>
+      <c r="DC98" s="6"/>
+      <c r="DD98" s="6"/>
       <c r="DE98" s="1"/>
-      <c r="DF98" s="5"/>
+      <c r="DF98" s="6"/>
       <c r="DG98" s="1"/>
-      <c r="DH98" s="5"/>
-      <c r="DI98" s="5"/>
+      <c r="DH98" s="6"/>
+      <c r="DI98" s="6"/>
       <c r="DJ98" s="1"/>
-      <c r="DK98" s="5"/>
+      <c r="DK98" s="6"/>
       <c r="DL98" s="1"/>
-      <c r="DM98" s="5"/>
-      <c r="DN98" s="5"/>
+      <c r="DM98" s="6"/>
+      <c r="DN98" s="6"/>
       <c r="DO98" s="1"/>
-      <c r="DP98" s="5"/>
+      <c r="DP98" s="6"/>
       <c r="DQ98" s="1"/>
-      <c r="DR98" s="5"/>
-      <c r="DS98" s="5"/>
+      <c r="DR98" s="6"/>
+      <c r="DS98" s="6"/>
       <c r="DT98" s="1"/>
-      <c r="DU98" s="5"/>
+      <c r="DU98" s="6"/>
       <c r="DV98" s="1"/>
-      <c r="DW98" s="5"/>
-      <c r="DX98" s="5"/>
+      <c r="DW98" s="6"/>
+      <c r="DX98" s="6"/>
       <c r="DY98" s="1"/>
-      <c r="DZ98" s="5"/>
+      <c r="DZ98" s="6"/>
       <c r="EA98" s="1"/>
-      <c r="EB98" s="5"/>
-      <c r="EC98" s="5"/>
+      <c r="EB98" s="6"/>
+      <c r="EC98" s="6"/>
       <c r="ED98" s="1"/>
-      <c r="EE98" s="5"/>
+      <c r="EE98" s="6"/>
       <c r="EF98" s="1"/>
-      <c r="EG98" s="5"/>
-      <c r="EH98" s="5"/>
+      <c r="EG98" s="6"/>
+      <c r="EH98" s="6"/>
       <c r="EI98" s="1"/>
-      <c r="EJ98" s="5"/>
+      <c r="EJ98" s="6"/>
       <c r="EK98" s="1"/>
-      <c r="EL98" s="5"/>
-      <c r="EM98" s="5"/>
+      <c r="EL98" s="6"/>
+      <c r="EM98" s="6"/>
       <c r="EN98" s="1"/>
-      <c r="EO98" s="5"/>
+      <c r="EO98" s="6"/>
       <c r="EP98" s="1"/>
-      <c r="EQ98" s="5"/>
-      <c r="ER98" s="5"/>
+      <c r="EQ98" s="6"/>
+      <c r="ER98" s="6"/>
       <c r="ES98" s="1"/>
-      <c r="ET98" s="5"/>
+      <c r="ET98" s="6"/>
       <c r="EU98" s="1"/>
-      <c r="EV98" s="5"/>
-      <c r="EW98" s="5"/>
+      <c r="EV98" s="6"/>
+      <c r="EW98" s="6"/>
       <c r="EX98" s="1"/>
-      <c r="EY98" s="5"/>
+      <c r="EY98" s="6"/>
       <c r="EZ98" s="1"/>
-      <c r="FA98" s="5"/>
-      <c r="FB98" s="5"/>
+      <c r="FA98" s="6"/>
+      <c r="FB98" s="6"/>
       <c r="FC98" s="1"/>
-      <c r="FD98" s="5"/>
+      <c r="FD98" s="6"/>
       <c r="FE98" s="1"/>
-      <c r="FF98" s="5"/>
-      <c r="FG98" s="5"/>
+      <c r="FF98" s="6"/>
+      <c r="FG98" s="6"/>
       <c r="FH98" s="1"/>
-      <c r="FI98" s="5"/>
+      <c r="FI98" s="6"/>
       <c r="FJ98" s="1"/>
-      <c r="FK98" s="5"/>
-      <c r="FL98" s="5"/>
+      <c r="FK98" s="6"/>
+      <c r="FL98" s="6"/>
       <c r="FM98" s="1"/>
-      <c r="FN98" s="5"/>
+      <c r="FN98" s="6"/>
       <c r="FO98" s="1"/>
-      <c r="FP98" s="5"/>
-      <c r="FQ98" s="5"/>
+      <c r="FP98" s="6"/>
+      <c r="FQ98" s="6"/>
       <c r="FR98" s="1"/>
-      <c r="FS98" s="5"/>
+      <c r="FS98" s="6"/>
       <c r="FT98" s="1"/>
-      <c r="FU98" s="5"/>
-      <c r="FV98" s="5"/>
+      <c r="FU98" s="6"/>
+      <c r="FV98" s="6"/>
       <c r="FW98" s="1"/>
-      <c r="FX98" s="5"/>
+      <c r="FX98" s="6"/>
       <c r="FY98" s="1"/>
-      <c r="FZ98" s="5"/>
-      <c r="GA98" s="5"/>
+      <c r="FZ98" s="6"/>
+      <c r="GA98" s="6"/>
       <c r="GB98" s="1"/>
-      <c r="GC98" s="5"/>
+      <c r="GC98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E101" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F101" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G101" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U101" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="1" t="n">
+        <f aca="false">B101*(PI()/5)</f>
+        <v>0</v>
+      </c>
+      <c r="C102" s="1" t="n">
+        <f aca="false">C101*(PI()/5)</f>
+        <v>0.628318530717959</v>
+      </c>
+      <c r="D102" s="1" t="n">
+        <f aca="false">D101*(PI()/5)</f>
+        <v>1.25663706143592</v>
+      </c>
+      <c r="E102" s="1" t="n">
+        <f aca="false">E101*(PI()/5)</f>
+        <v>1.88495559215388</v>
+      </c>
+      <c r="F102" s="1" t="n">
+        <f aca="false">F101*(PI()/5)</f>
+        <v>2.51327412287183</v>
+      </c>
+      <c r="G102" s="1" t="n">
+        <f aca="false">G101*(PI()/5)</f>
+        <v>3.14159265358979</v>
+      </c>
+      <c r="N102" s="1" t="n">
+        <f aca="false">PI()/10</f>
+        <v>0.314159265358979</v>
+      </c>
+      <c r="O102" s="1" t="n">
+        <f aca="false">PI()/5</f>
+        <v>0.628318530717959</v>
+      </c>
+      <c r="R102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S102" s="1" t="n">
+        <f aca="false">$N$4*(SIN(C102)-SIN(B102))/2+SIN(B102)*$N$4</f>
+        <v>0.0923290915245227</v>
+      </c>
+      <c r="T102" s="2" t="n">
+        <f aca="false">S102/$O$4</f>
+        <v>0.293892626146237</v>
+      </c>
+      <c r="U102" s="3" t="n">
+        <f aca="false">T102*$O$6</f>
+        <v>2938.92626146237</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="1" t="n">
+        <f aca="false">SIN(B102)</f>
+        <v>0</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <f aca="false">SIN(C102)</f>
+        <v>0.587785252292473</v>
+      </c>
+      <c r="D103" s="1" t="n">
+        <f aca="false">SIN(D102)</f>
+        <v>0.951056516295154</v>
+      </c>
+      <c r="E103" s="1" t="n">
+        <f aca="false">SIN(E102)</f>
+        <v>0.951056516295154</v>
+      </c>
+      <c r="F103" s="1" t="n">
+        <f aca="false">SIN(F102)</f>
+        <v>0.587785252292473</v>
+      </c>
+      <c r="G103" s="1" t="n">
+        <f aca="false">SIN(G102)</f>
+        <v>1.22464679914735E-016</v>
+      </c>
+      <c r="R103" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S103" s="1" t="n">
+        <f aca="false">$N$4*(SIN(D102)-SIN(C102))/2+SIN(C102)*$N$4</f>
+        <v>0.2417206997616</v>
+      </c>
+      <c r="T103" s="2" t="n">
+        <f aca="false">S103/$O$4</f>
+        <v>0.769420884293813</v>
+      </c>
+      <c r="U103" s="3" t="n">
+        <f aca="false">T103*$O$6</f>
+        <v>7694.20884293813</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="1" t="n">
+        <f aca="false">COS(B102)-COS(C102)</f>
+        <v>0.190983005625053</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <f aca="false">COS(C102)-COS(D102)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D104" s="1" t="n">
+        <f aca="false">COS(D102)-COS(E102)</f>
+        <v>0.618033988749895</v>
+      </c>
+      <c r="E104" s="1" t="n">
+        <f aca="false">COS(E102)-COS(F102)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F104" s="1" t="n">
+        <f aca="false">COS(F102)-COS(G102)</f>
+        <v>0.190983005625053</v>
+      </c>
+      <c r="G104" s="1" t="n">
+        <f aca="false">COS(G102)-(-1)</f>
+        <v>0</v>
+      </c>
+      <c r="N104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O104" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R104" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="S104" s="1" t="n">
+        <f aca="false">$N$4*(SIN(E102)-SIN(D102))/2+SIN(D102)*$N$4</f>
+        <v>0.298783216474155</v>
+      </c>
+      <c r="T104" s="2" t="n">
+        <f aca="false">S104/$O$4</f>
+        <v>0.951056516295153</v>
+      </c>
+      <c r="U104" s="3" t="n">
+        <f aca="false">T104*$O$6</f>
+        <v>9510.56516295153</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B105" s="2" t="n">
+        <f aca="false">B104/$O$102</f>
+        <v>0.303958893917744</v>
+      </c>
+      <c r="C105" s="2" t="n">
+        <f aca="false">C104/$O$102</f>
+        <v>0.795774715459477</v>
+      </c>
+      <c r="D105" s="2" t="n">
+        <f aca="false">D104/$O$102</f>
+        <v>0.983631643083466</v>
+      </c>
+      <c r="E105" s="2" t="n">
+        <f aca="false">E104/$O$102</f>
+        <v>0.795774715459477</v>
+      </c>
+      <c r="F105" s="2" t="n">
+        <f aca="false">F104/$O$102</f>
+        <v>0.303958893917744</v>
+      </c>
+      <c r="G105" s="2" t="n">
+        <f aca="false">G104/$O$102</f>
+        <v>0</v>
+      </c>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="L105" s="2"/>
+      <c r="N105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O105" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="R105" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="S105" s="1" t="n">
+        <f aca="false">$N$4*(SIN(F102)-SIN(E102))/2+SIN(E102)*$N$4</f>
+        <v>0.2417206997616</v>
+      </c>
+      <c r="T105" s="2" t="n">
+        <f aca="false">S105/$O$4</f>
+        <v>0.769420884293814</v>
+      </c>
+      <c r="U105" s="3" t="n">
+        <f aca="false">T105*$O$6</f>
+        <v>7694.20884293814</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O106" s="1" t="n">
+        <f aca="false">1/(2*PI()*O105)</f>
+        <v>0.00318309886183791</v>
+      </c>
+      <c r="R106" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S106" s="1" t="n">
+        <f aca="false">$N$4*(SIN(G102)-SIN(F102))/2+SIN(F102)*$N$4</f>
+        <v>0.0923290915245228</v>
+      </c>
+      <c r="T106" s="2" t="n">
+        <f aca="false">S106/$O$4</f>
+        <v>0.293892626146237</v>
+      </c>
+      <c r="U106" s="3" t="n">
+        <f aca="false">T106*$O$6</f>
+        <v>2938.92626146237</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F107" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G107" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="N107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O107" s="1" t="n">
+        <f aca="false">O106/10000</f>
+        <v>3.18309886183791E-007</v>
+      </c>
+      <c r="P107" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R107" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S107" s="1" t="n">
+        <f aca="false">$N$4*(SIN(H102)-SIN(G102))/2+SIN(G102)*$N$4</f>
+        <v>1.92367069372179E-017</v>
+      </c>
+      <c r="T107" s="2" t="n">
+        <f aca="false">S107/$O$4</f>
+        <v>6.12323399573677E-017</v>
+      </c>
+      <c r="U107" s="3" t="n">
+        <f aca="false">T107*$O$6</f>
+        <v>6.12323399573677E-013</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="3" t="n">
+        <f aca="false">B105*$O$104</f>
+        <v>1519.79446958872</v>
+      </c>
+      <c r="C108" s="3" t="n">
+        <f aca="false">C105*$O$104</f>
+        <v>3978.87357729738</v>
+      </c>
+      <c r="D108" s="3" t="n">
+        <f aca="false">D105*$O$104</f>
+        <v>4918.15821541733</v>
+      </c>
+      <c r="E108" s="3" t="n">
+        <f aca="false">E105*$O$104</f>
+        <v>3978.87357729738</v>
+      </c>
+      <c r="F108" s="3" t="n">
+        <f aca="false">F105*$O$104</f>
+        <v>1519.79446958872</v>
+      </c>
+      <c r="G108" s="3" t="n">
+        <f aca="false">G105*$O$104</f>
+        <v>0</v>
+      </c>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="N108" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O108" s="1" t="n">
+        <f aca="false">10000*0.000047</f>
+        <v>0.47</v>
+      </c>
+      <c r="R108" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="S108" s="1" t="n">
+        <f aca="false">$N$4*(SIN(I102)-SIN(H102))/2+SIN(H102)*$N$4</f>
+        <v>0</v>
+      </c>
+      <c r="T108" s="2" t="n">
+        <f aca="false">S108/$O$4</f>
+        <v>0</v>
+      </c>
+      <c r="U108" s="3" t="n">
+        <f aca="false">T108*$O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O109" s="1" t="n">
+        <f aca="false">1/O108</f>
+        <v>2.12765957446809</v>
+      </c>
+      <c r="R109" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S109" s="1" t="n">
+        <f aca="false">$N$4*(SIN(J102)-SIN(I102))/2+SIN(I102)*$N$4</f>
+        <v>0</v>
+      </c>
+      <c r="T109" s="2" t="n">
+        <f aca="false">S109/$O$4</f>
+        <v>0</v>
+      </c>
+      <c r="U109" s="3" t="n">
+        <f aca="false">T109*$O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R110" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="S110" s="1" t="n">
+        <f aca="false">$N$4*(SIN(K102)-SIN(J102))/2+SIN(J102)*$N$4</f>
+        <v>0</v>
+      </c>
+      <c r="T110" s="2" t="n">
+        <f aca="false">S110/$O$4</f>
+        <v>0</v>
+      </c>
+      <c r="U110" s="3" t="n">
+        <f aca="false">T110*$O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R111" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="S111" s="1" t="n">
+        <f aca="false">$N$4*(SIN(L102)-SIN(K102))/2+SIN(K102)*$N$4</f>
+        <v>0</v>
+      </c>
+      <c r="T111" s="2" t="n">
+        <f aca="false">S111/$O$4</f>
+        <v>0</v>
+      </c>
+      <c r="U111" s="3" t="n">
+        <f aca="false">T111*$O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="1" t="str">
+        <f aca="false">B106</f>
+        <v>Intervalo 1</v>
+      </c>
+      <c r="C143" s="2" t="n">
+        <f aca="false">B105</f>
+        <v>0.303958893917744</v>
+      </c>
+      <c r="D143" s="1" t="n">
+        <f aca="false">C143*100</f>
+        <v>30.3958893917744</v>
+      </c>
+      <c r="M143" s="1"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C144" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D144" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E144" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F144" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G144" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D145" s="1" t="n">
+        <f aca="false">D143-20</f>
+        <v>10.3958893917744</v>
+      </c>
+      <c r="E145" s="1" t="n">
+        <f aca="false">D145-20</f>
+        <v>-9.60411060822563</v>
+      </c>
+      <c r="F145" s="1" t="n">
+        <f aca="false">E145-20</f>
+        <v>-29.6041106082256</v>
+      </c>
+      <c r="G145" s="1" t="n">
+        <f aca="false">F145-20</f>
+        <v>-49.6041106082256</v>
+      </c>
+      <c r="M145" s="1"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C146" s="5" t="n">
+        <f aca="false">IF(D143&gt;20,100,D143)</f>
+        <v>100</v>
+      </c>
+      <c r="D146" s="5" t="n">
+        <f aca="false">IF(D145&gt;20,100,IF(D145&lt;0,0,D145*10))</f>
+        <v>103.958893917744</v>
+      </c>
+      <c r="E146" s="5" t="n">
+        <f aca="false">IF(E145&gt;10,100,IF(E145&lt;0,0,E145*10))</f>
+        <v>0</v>
+      </c>
+      <c r="F146" s="5" t="n">
+        <f aca="false">IF(F145&gt;10,100,IF(F145&lt;0,0,F145*10))</f>
+        <v>0</v>
+      </c>
+      <c r="G146" s="5" t="n">
+        <f aca="false">IF(G145&gt;10,100,IF(G145&lt;0,0,G145*10))</f>
+        <v>0</v>
+      </c>
+      <c r="H146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="J146" s="5"/>
+      <c r="K146" s="5"/>
+      <c r="L146" s="5"/>
+      <c r="M146" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="1" t="str">
+        <f aca="false">C106</f>
+        <v>Intervalo 2</v>
+      </c>
+      <c r="C149" s="2" t="n">
+        <f aca="false">C105</f>
+        <v>0.795774715459477</v>
+      </c>
+      <c r="D149" s="1" t="n">
+        <f aca="false">C149*100</f>
+        <v>79.5774715459477</v>
+      </c>
+      <c r="M149" s="1"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D150" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E150" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F150" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G150" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D151" s="1" t="n">
+        <f aca="false">D149-20</f>
+        <v>59.5774715459477</v>
+      </c>
+      <c r="E151" s="1" t="n">
+        <f aca="false">D151-20</f>
+        <v>39.5774715459477</v>
+      </c>
+      <c r="F151" s="1" t="n">
+        <f aca="false">E151-20</f>
+        <v>19.5774715459477</v>
+      </c>
+      <c r="G151" s="1" t="n">
+        <f aca="false">F151-20</f>
+        <v>-0.422528454052326</v>
+      </c>
+      <c r="N151" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O151" s="1" t="e">
+        <f aca="false">1/(2*PI()*O150)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R151" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="5" t="n">
+        <f aca="false">IF(D149&gt;10,100,D149)</f>
+        <v>100</v>
+      </c>
+      <c r="D152" s="5" t="n">
+        <f aca="false">IF(D151&gt;10,100,IF(D151&lt;0,0,D151*10))</f>
+        <v>100</v>
+      </c>
+      <c r="E152" s="5" t="n">
+        <f aca="false">IF(E151&gt;10,100,IF(E151&lt;0,0,E151*10))</f>
+        <v>100</v>
+      </c>
+      <c r="F152" s="5" t="n">
+        <f aca="false">IF(F151&gt;10,100,IF(F151&lt;0,0,F151*10))</f>
+        <v>100</v>
+      </c>
+      <c r="G152" s="5" t="n">
+        <f aca="false">IF(G151&gt;10,100,IF(G151&lt;0,0,G151*10))</f>
+        <v>0</v>
+      </c>
+      <c r="N152" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O152" s="1" t="e">
+        <f aca="false">O151/10000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P152" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R152" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G153" s="3"/>
+      <c r="H153" s="3"/>
+      <c r="I153" s="3"/>
+      <c r="J153" s="3"/>
+      <c r="K153" s="3"/>
+      <c r="L153" s="3"/>
+      <c r="N153" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O153" s="1" t="n">
+        <f aca="false">10000*0.000047</f>
+        <v>0.47</v>
+      </c>
+      <c r="R153" s="1" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O154" s="1" t="n">
+        <f aca="false">1/O153</f>
+        <v>2.12765957446809</v>
+      </c>
+      <c r="R154" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="1" t="str">
+        <f aca="false">D106</f>
+        <v>Intervalo 3</v>
+      </c>
+      <c r="C155" s="2" t="n">
+        <f aca="false">D105</f>
+        <v>0.983631643083466</v>
+      </c>
+      <c r="D155" s="1" t="n">
+        <f aca="false">C155*100</f>
+        <v>98.3631643083466</v>
+      </c>
+      <c r="M155" s="1"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C156" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D156" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E156" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F156" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G156" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D157" s="1" t="n">
+        <f aca="false">D155-10</f>
+        <v>88.3631643083466</v>
+      </c>
+      <c r="E157" s="1" t="n">
+        <f aca="false">D157-10</f>
+        <v>78.3631643083466</v>
+      </c>
+      <c r="F157" s="1" t="n">
+        <f aca="false">E157-10</f>
+        <v>68.3631643083466</v>
+      </c>
+      <c r="G157" s="1" t="n">
+        <f aca="false">F157-10</f>
+        <v>58.3631643083466</v>
+      </c>
+      <c r="M157" s="1"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="5" t="n">
+        <f aca="false">IF(D155&gt;10,100,D155)</f>
+        <v>100</v>
+      </c>
+      <c r="D158" s="5" t="n">
+        <f aca="false">IF(D157&gt;10,100,IF(D157&lt;0,0,D157*10))</f>
+        <v>100</v>
+      </c>
+      <c r="E158" s="5" t="n">
+        <f aca="false">IF(E157&gt;10,100,IF(E157&lt;0,0,E157*10))</f>
+        <v>100</v>
+      </c>
+      <c r="F158" s="5" t="n">
+        <f aca="false">IF(F157&gt;10,100,IF(F157&lt;0,0,F157*10))</f>
+        <v>100</v>
+      </c>
+      <c r="G158" s="5" t="n">
+        <f aca="false">IF(G157&gt;10,100,IF(G157&lt;0,0,G157*10))</f>
+        <v>100</v>
+      </c>
+      <c r="H158" s="5"/>
+      <c r="I158" s="5"/>
+      <c r="J158" s="5"/>
+      <c r="K158" s="5"/>
+      <c r="L158" s="5"/>
+      <c r="M158" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="1" t="str">
+        <f aca="false">E106</f>
+        <v>Intervalo 4</v>
+      </c>
+      <c r="C161" s="2" t="n">
+        <f aca="false">E105</f>
+        <v>0.795774715459477</v>
+      </c>
+      <c r="D161" s="1" t="n">
+        <f aca="false">C161*100</f>
+        <v>79.5774715459477</v>
+      </c>
+      <c r="M161" s="1"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B162" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C162" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D162" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E162" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F162" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G162" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="M162" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D163" s="1" t="n">
+        <f aca="false">D161-10</f>
+        <v>69.5774715459477</v>
+      </c>
+      <c r="E163" s="1" t="n">
+        <f aca="false">D163-10</f>
+        <v>59.5774715459477</v>
+      </c>
+      <c r="F163" s="1" t="n">
+        <f aca="false">E163-10</f>
+        <v>49.5774715459477</v>
+      </c>
+      <c r="G163" s="1" t="n">
+        <f aca="false">F163-10</f>
+        <v>39.5774715459477</v>
+      </c>
+      <c r="M163" s="1"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="5" t="n">
+        <f aca="false">IF(D161&gt;10,100,D161)</f>
+        <v>100</v>
+      </c>
+      <c r="D164" s="5" t="n">
+        <f aca="false">IF(D163&gt;10,100,IF(D163&lt;0,0,D163*10))</f>
+        <v>100</v>
+      </c>
+      <c r="E164" s="5" t="n">
+        <f aca="false">IF(E163&gt;10,100,IF(E163&lt;0,0,E163*10))</f>
+        <v>100</v>
+      </c>
+      <c r="F164" s="5" t="n">
+        <f aca="false">IF(F163&gt;10,100,IF(F163&lt;0,0,F163*10))</f>
+        <v>100</v>
+      </c>
+      <c r="G164" s="5" t="n">
+        <f aca="false">IF(G163&gt;10,100,IF(G163&lt;0,0,G163*10))</f>
+        <v>100</v>
+      </c>
+      <c r="H164" s="5"/>
+      <c r="I164" s="5"/>
+      <c r="J164" s="5"/>
+      <c r="K164" s="5"/>
+      <c r="L164" s="5"/>
+      <c r="M164" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="1" t="str">
+        <f aca="false">F106</f>
+        <v>Intervalo 5</v>
+      </c>
+      <c r="C167" s="2" t="n">
+        <f aca="false">F105</f>
+        <v>0.303958893917744</v>
+      </c>
+      <c r="D167" s="1" t="n">
+        <f aca="false">C167*100</f>
+        <v>30.3958893917744</v>
+      </c>
+      <c r="M167" s="1"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C168" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D168" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E168" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F168" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G168" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="M168" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D169" s="1" t="n">
+        <f aca="false">D167-10</f>
+        <v>20.3958893917744</v>
+      </c>
+      <c r="E169" s="1" t="n">
+        <f aca="false">D169-10</f>
+        <v>10.3958893917744</v>
+      </c>
+      <c r="F169" s="1" t="n">
+        <f aca="false">E169-10</f>
+        <v>0.395889391774382</v>
+      </c>
+      <c r="G169" s="1" t="n">
+        <f aca="false">F169-10</f>
+        <v>-9.60411060822562</v>
+      </c>
+      <c r="M169" s="1"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="5" t="n">
+        <f aca="false">IF(D167&gt;10,100,D167)</f>
+        <v>100</v>
+      </c>
+      <c r="D170" s="5" t="n">
+        <f aca="false">IF(D169&gt;10,100,IF(D169&lt;0,0,D169*10))</f>
+        <v>100</v>
+      </c>
+      <c r="E170" s="5" t="n">
+        <f aca="false">IF(E169&gt;10,100,IF(E169&lt;0,0,E169*10))</f>
+        <v>100</v>
+      </c>
+      <c r="F170" s="5" t="n">
+        <f aca="false">IF(F169&gt;10,100,IF(F169&lt;0,0,F169*10))</f>
+        <v>3.95889391774382</v>
+      </c>
+      <c r="G170" s="5" t="n">
+        <f aca="false">IF(G169&gt;10,100,IF(G169&lt;0,0,G169*10))</f>
+        <v>0</v>
+      </c>
+      <c r="H170" s="5"/>
+      <c r="I170" s="5"/>
+      <c r="J170" s="5"/>
+      <c r="K170" s="5"/>
+      <c r="L170" s="5"/>
+      <c r="M170" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="1" t="str">
+        <f aca="false">G106</f>
+        <v>Intervalo 6</v>
+      </c>
+      <c r="C173" s="2" t="n">
+        <f aca="false">G105</f>
+        <v>0</v>
+      </c>
+      <c r="D173" s="1" t="n">
+        <f aca="false">C173*100</f>
+        <v>0</v>
+      </c>
+      <c r="M173" s="1"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C174" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D174" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E174" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F174" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="G174" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D175" s="1" t="n">
+        <f aca="false">D173-10</f>
+        <v>-10</v>
+      </c>
+      <c r="E175" s="1" t="n">
+        <f aca="false">D175-10</f>
+        <v>-20</v>
+      </c>
+      <c r="F175" s="1" t="n">
+        <f aca="false">E175-10</f>
+        <v>-30</v>
+      </c>
+      <c r="G175" s="1" t="n">
+        <f aca="false">F175-10</f>
+        <v>-40</v>
+      </c>
+      <c r="M175" s="1"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C176" s="5" t="n">
+        <f aca="false">IF(D173&gt;10,100,D173)</f>
+        <v>0</v>
+      </c>
+      <c r="D176" s="5" t="n">
+        <f aca="false">IF(D175&gt;10,100,IF(D175&lt;0,0,D175*10))</f>
+        <v>0</v>
+      </c>
+      <c r="E176" s="5" t="n">
+        <f aca="false">IF(E175&gt;10,100,IF(E175&lt;0,0,E175*10))</f>
+        <v>0</v>
+      </c>
+      <c r="F176" s="5" t="n">
+        <f aca="false">IF(F175&gt;10,100,IF(F175&lt;0,0,F175*10))</f>
+        <v>0</v>
+      </c>
+      <c r="G176" s="5" t="n">
+        <f aca="false">IF(G175&gt;10,100,IF(G175&lt;0,0,G175*10))</f>
+        <v>0</v>
+      </c>
+      <c r="H176" s="5"/>
+      <c r="I176" s="5"/>
+      <c r="J176" s="5"/>
+      <c r="K176" s="5"/>
+      <c r="L176" s="5"/>
+      <c r="M176" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>